<commit_message>
Update SQL pathc script and other sources
</commit_message>
<xml_diff>
--- a/php/#docs/WarQuest buildings.xlsx
+++ b/php/#docs/WarQuest buildings.xlsx
@@ -702,25 +702,25 @@
     <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="12" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="14" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="13" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="7" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="10" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Kop 1" xfId="3" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="4" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="5" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="6" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="9" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="16" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="8" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="18" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="17" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="15" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,9 +728,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -768,7 +768,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -838,7 +838,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B245" sqref="B245"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>